<commit_message>
Enrich Data Frame with more Data
* add google trends Interface
* add milk prices
* add yogurt prices
* clean up prophet model with regressors
</commit_message>
<xml_diff>
--- a/data_hs21/milchpreis.xlsx
+++ b/data_hs21/milchpreis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hahn\Documents\Master\temp\test\yogurt-prediction\data_hs21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9694606D-34E8-4C9B-8493-ED996334123F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F750BB-CEF5-4BA3-B94A-41F696E179F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33990" yWindow="3150" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -231,7 +231,7 @@
     <t>07.21</t>
   </si>
   <si>
-    <t>prod-milchpreis-a</t>
+    <t>prod.milchpreis.a</t>
   </si>
 </sst>
 </file>
@@ -611,13 +611,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -625,7 +625,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -633,7 +633,7 @@
         <v>61.888851927264732</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -641,7 +641,7 @@
         <v>59.732856620889002</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -649,7 +649,7 @@
         <v>59.385609588549791</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -657,7 +657,7 @@
         <v>56.190004597172418</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -665,7 +665,7 @@
         <v>56.18945397402274</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -673,7 +673,7 @@
         <v>55.292906931222596</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -681,7 +681,7 @@
         <v>57.200697606672612</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -689,7 +689,7 @@
         <v>58.21342927886181</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -697,7 +697,7 @@
         <v>58.709287768633047</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -705,7 +705,7 @@
         <v>60.272423204915292</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -713,7 +713,7 @@
         <v>59.035858249958288</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -721,7 +721,7 @@
         <v>58.887041634950869</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -729,7 +729,7 @@
         <v>59.545304983605249</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -737,7 +737,7 @@
         <v>57.290952268200272</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -745,7 +745,7 @@
         <v>56.341575565671363</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -753,7 +753,7 @@
         <v>56.679519614438952</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -761,7 +761,7 @@
         <v>56.589807852595605</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -769,7 +769,7 @@
         <v>57.296254390282954</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -777,7 +777,7 @@
         <v>59.893586238332276</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -785,7 +785,7 @@
         <v>60.495874140242201</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -793,7 +793,7 @@
         <v>62.124996791474658</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -801,7 +801,7 @@
         <v>65.820780431562184</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -809,7 +809,7 @@
         <v>65.77880348661408</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -817,7 +817,7 @@
         <v>65.08090431470103</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -825,7 +825,7 @@
         <v>63.998227324914239</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -833,7 +833,7 @@
         <v>62.232504147459231</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -841,7 +841,7 @@
         <v>60.683576219834563</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -849,7 +849,7 @@
         <v>60.083074107425595</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -857,7 +857,7 @@
         <v>59.029622298015987</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -865,7 +865,7 @@
         <v>60.754704583322507</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -873,7 +873,7 @@
         <v>61.828100121879771</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -881,7 +881,7 @@
         <v>62.544489616958025</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -889,7 +889,7 @@
         <v>63.755011560538705</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -897,7 +897,7 @@
         <v>64.053031154241481</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -905,7 +905,7 @@
         <v>63.302392831926994</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -913,7 +913,7 @@
         <v>63.279310569711598</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -921,7 +921,7 @@
         <v>63.185012680069619</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -929,7 +929,7 @@
         <v>59.759433436608155</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -937,7 +937,7 @@
         <v>58.810362521372191</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -945,7 +945,7 @@
         <v>58.517101631812388</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -953,7 +953,7 @@
         <v>58.365483298241088</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -961,7 +961,7 @@
         <v>60.124250430183338</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -969,7 +969,7 @@
         <v>61.585168927612102</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -977,7 +977,7 @@
         <v>64.575169229819565</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -985,7 +985,7 @@
         <v>67.219160361571966</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -993,7 +993,7 @@
         <v>68.781227771965447</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>67.237744568862837</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>66.899951143263195</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>66.465227152600249</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>64.232753816768707</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>63.908429928339302</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>63.488607757183061</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>63.287013787330253</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>64.611655239380951</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>66.515339614176526</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>67.258805707111605</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>67.650912551682964</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>68.625026028631851</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>66.334395363507866</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>66.64219230828553</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>69.102027121194666</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>67.667990785995912</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>67.010000000000005</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>66.180000000000007</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>66.150000000000006</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>68.260000000000005</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>

</xml_diff>